<commit_message>
Creacion Funcion GetParameter - Quitado comprobantes a desestimar Solapa Objetivos Facturacion
</commit_message>
<xml_diff>
--- a/DBA/Reportes BI/2021/Facturación/Efectores.xlsx
+++ b/DBA/Reportes BI/2021/Facturación/Efectores.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iachenbach\Desktop\FACOEP\DBA\Reportes BI\2021\Facturación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iachenbach\Gobierno de la Ciudad de Buenos Aires\Pablo Alfredo Gadea - Tablero Facoep P BI\FACOEP\DBA\Reportes BI\2021\Facturación\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>sif</t>
   </si>
@@ -140,18 +140,12 @@
     <t xml:space="preserve">EFECTORES EXTRAHOSPITALARIOS            </t>
   </si>
   <si>
-    <t>Efector</t>
-  </si>
-  <si>
     <t>Barrio 31</t>
   </si>
   <si>
     <t>Lagleyze</t>
   </si>
   <si>
-    <t>Grrierson</t>
-  </si>
-  <si>
     <t>Santojanni</t>
   </si>
   <si>
@@ -230,9 +224,6 @@
     <t>Sardá</t>
   </si>
   <si>
-    <t>Marie Curie</t>
-  </si>
-  <si>
     <t>Quemados</t>
   </si>
   <si>
@@ -245,20 +236,32 @@
     <t>Tobar García</t>
   </si>
   <si>
-    <t>Talleres Protegidos</t>
-  </si>
-  <si>
     <t>Borda</t>
   </si>
   <si>
     <t>Turismo</t>
+  </si>
+  <si>
+    <t>Grierson</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>EfectorObjetivos</t>
+  </si>
+  <si>
+    <t>Maria Curie</t>
+  </si>
+  <si>
+    <t>Talleres protegidos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -266,16 +269,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -283,12 +313,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -307,11 +353,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:B38" totalsRowShown="0">
-  <autoFilter ref="A1:B38"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:C38" totalsRowShown="0">
+  <autoFilter ref="A1:C38"/>
+  <sortState ref="A2:C38">
+    <sortCondition ref="A1:A38"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="3" name="ID"/>
     <tableColumn id="1" name="sif"/>
-    <tableColumn id="2" name="Efector"/>
+    <tableColumn id="2" name="EfectorObjetivos"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -580,320 +630,435 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.5703125" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="57.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>424</v>
+      </c>
+      <c r="B26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>425</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>702</v>
+      </c>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>704</v>
+      </c>
+      <c r="B29" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>938</v>
+      </c>
+      <c r="B30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1466</v>
+      </c>
+      <c r="B31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1607</v>
+      </c>
+      <c r="B32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1644</v>
+      </c>
+      <c r="B33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1855</v>
+      </c>
+      <c r="B34" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>2334</v>
+      </c>
+      <c r="B35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>2678</v>
+      </c>
+      <c r="B36" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>3118</v>
+      </c>
+      <c r="B37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="H37" s="3"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>3140</v>
+      </c>
+      <c r="B38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>36</v>
-      </c>
-      <c r="B38" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>